<commit_message>
Se realizarón cambios al plan de pruebas
</commit_message>
<xml_diff>
--- a/RecursosPokeDexApp/MetricaPokeDex.xlsx
+++ b/RecursosPokeDexApp/MetricaPokeDex.xlsx
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geova\OneDrive\Escritorio\PokeDexApp\PokeDexPruebas\RecursosPokeDexApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25357290-D5BC-4E20-AD4D-5E5108081143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B689F32-954F-4509-8994-2DDA7D4E8625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07B3B8C5-F78C-4A40-A48E-EB7C2DCE21A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Hoja1!$C$15:$C$21</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Hoja1!$D$15:$D$21</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Hoja1!$C$15:$C$21</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Hoja1!$D$15:$D$21</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -510,12 +504,6 @@
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,6 +579,12 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Énfasis4" xfId="2" builtinId="42"/>
@@ -599,20 +593,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -664,13 +644,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -686,7 +659,25 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -726,6 +717,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1813,37 +1807,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}" name="Tabla1" displayName="Tabla1" ref="C5:P10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}" name="Tabla1" displayName="Tabla1" ref="C5:P10" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="C5:P10" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{CE661E64-349B-4503-8826-B72573538F9D}" name="Equipo" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{47D53C6E-257D-4D3F-8519-A3EAC8E06F0A}" name="No. Ticket" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{04FEA45B-8C42-420B-9EFE-B8E9DCB21DAF}" name="Develper" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{E05212F3-297D-4B2E-B7BB-603C1557FD5E}" name="QA" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{6DC710F3-E776-46E8-8F84-EC7ACEEA88AE}" name="Errores" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{CE661E64-349B-4503-8826-B72573538F9D}" name="Equipo" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{47D53C6E-257D-4D3F-8519-A3EAC8E06F0A}" name="No. Ticket" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{04FEA45B-8C42-420B-9EFE-B8E9DCB21DAF}" name="Develper" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{E05212F3-297D-4B2E-B7BB-603C1557FD5E}" name="QA" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{6DC710F3-E776-46E8-8F84-EC7ACEEA88AE}" name="Errores" dataDxfId="15">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3251B65F-8616-458F-8314-BDFE7400D956}" name="Funcionalidad " dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{4B3D8399-75D5-4FFF-82B9-643CFC3BF2F3}" name="UI/UX" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{BA62243D-765A-4990-8932-8BD998D4DA23}" name="Rendimiento" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{EF6BB8C3-FC2D-4677-BBFD-233798FD9208}" name="Usabilidad " dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{23AEB557-49E9-4C99-8DE0-1A2D9022BA2A}" name="DB" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{1C766899-B3D1-48D7-B4E8-007A9E9507FF}" name="Seguridad" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{5DF6092B-CA5C-4360-9B0F-BA2B1171C425}" name="Regresión " dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{A0CDFA20-32E7-44FF-B1F9-30AF643CF95F}" name="Casos de prueba/Estrategia" dataDxfId="11" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="14" xr3:uid="{F2EF59F0-F662-4015-A221-5F8D73430C76}" name="FeedBack" dataDxfId="10" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{3251B65F-8616-458F-8314-BDFE7400D956}" name="Funcionalidad " dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{4B3D8399-75D5-4FFF-82B9-643CFC3BF2F3}" name="UI/UX" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{BA62243D-765A-4990-8932-8BD998D4DA23}" name="Rendimiento" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{EF6BB8C3-FC2D-4677-BBFD-233798FD9208}" name="Usabilidad " dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{23AEB557-49E9-4C99-8DE0-1A2D9022BA2A}" name="DB" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{1C766899-B3D1-48D7-B4E8-007A9E9507FF}" name="Seguridad" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{5DF6092B-CA5C-4360-9B0F-BA2B1171C425}" name="Regresión " dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{A0CDFA20-32E7-44FF-B1F9-30AF643CF95F}" name="Casos de prueba/Estrategia" dataDxfId="7" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="14" xr3:uid="{F2EF59F0-F662-4015-A221-5F8D73430C76}" name="FeedBack" dataDxfId="6" dataCellStyle="Hipervínculo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}" name="Tabla2" displayName="Tabla2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}" name="Tabla2" displayName="Tabla2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="F14:H19" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{49D17C54-4FBB-4EEB-9308-81ECD18F5D70}" name="Developer" dataDxfId="3" dataCellStyle="20% - Énfasis4"/>
-    <tableColumn id="2" xr3:uid="{BCB2DB60-3C65-4281-BC4B-E0A4D451DB4F}" name="Cantidad de Arreglos" dataDxfId="2" dataCellStyle="20% - Énfasis4"/>
-    <tableColumn id="3" xr3:uid="{85195C94-0866-4075-B0A8-863518C19B56}" name="Lineas de codigo" dataDxfId="1" dataCellStyle="20% - Énfasis4"/>
+    <tableColumn id="1" xr3:uid="{49D17C54-4FBB-4EEB-9308-81ECD18F5D70}" name="Developer" dataDxfId="2" dataCellStyle="20% - Énfasis4"/>
+    <tableColumn id="2" xr3:uid="{BCB2DB60-3C65-4281-BC4B-E0A4D451DB4F}" name="Cantidad de Arreglos" dataDxfId="1" dataCellStyle="20% - Énfasis4"/>
+    <tableColumn id="3" xr3:uid="{85195C94-0866-4075-B0A8-863518C19B56}" name="Lineas de codigo" dataDxfId="0" dataCellStyle="20% - Énfasis4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2148,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8C6C0E-0565-4237-84BC-4574154DDE1B}">
   <dimension ref="C1:R21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,157 +2158,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="3:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="C3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
         <v>10</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>8</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5" t="s">
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="1" t="s">
@@ -2325,47 +2319,47 @@
       </c>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
         <v>11</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>7</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>3</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5" t="s">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="Q7" s="1" t="s">
@@ -2373,47 +2367,47 @@
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>3</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
         <v>14</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <v>11</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>3</v>
       </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5" t="s">
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -2421,47 +2415,47 @@
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
         <v>5</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>3</v>
       </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5" t="s">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="Q9" s="1" t="s">
@@ -2469,47 +2463,47 @@
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
         <v>14</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="2">
         <v>11</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>2</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="2">
         <v>1</v>
       </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Q10" s="1" t="s">
@@ -2517,245 +2511,245 @@
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="26" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="19">
         <f>SUM(Tabla1[[Funcionalidad ]])</f>
         <v>39</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="20">
         <f>SUM(Tabla1[UI/UX])</f>
         <v>13</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="20">
         <f>SUM(Tabla1[Rendimiento])</f>
         <v>2</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="20">
         <f>SUM(Tabla1[[Usabilidad ]])</f>
         <v>0</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="20">
         <f>SUM(Tabla1[DB])</f>
         <v>0</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="20">
         <f>SUM(Tabla1[Seguridad])</f>
         <v>0</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="21">
         <f>SUM(Tabla1[[Regresión ]])</f>
         <v>0</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se realizaron cambios al documento de metricas de QA
</commit_message>
<xml_diff>
--- a/RecursosPokeDexApp/MetricaPokeDex.xlsx
+++ b/RecursosPokeDexApp/MetricaPokeDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geova\OneDrive\Escritorio\PokeDexApp\PokeDexPruebas\RecursosPokeDexApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B689F32-954F-4509-8994-2DDA7D4E8625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17766EF7-3E15-40AF-AAA3-DD101B751439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07B3B8C5-F78C-4A40-A48E-EB7C2DCE21A2}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>Cantidad de Arreglos</t>
   </si>
   <si>
-    <t>Lineas de codigo</t>
-  </si>
-  <si>
     <t>Funcional</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Regreción</t>
+  </si>
+  <si>
+    <t>Cantidad de errores</t>
   </si>
 </sst>
 </file>
@@ -210,15 +210,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -231,6 +222,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Showcard Gothic"/>
+      <family val="5"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -270,17 +268,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -492,6 +479,39 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -501,7 +521,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -510,22 +530,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
@@ -537,52 +545,55 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -774,7 +785,7 @@
                     </a:prstClr>
                   </a:outerShdw>
                 </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -793,7 +804,7 @@
                     </a:prstClr>
                   </a:outerShdw>
                 </a:effectLst>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
               </a:rPr>
               <a:t>Grafico De Errores</a:t>
             </a:r>
@@ -826,7 +837,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -931,7 +942,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$C$15:$C$21</c:f>
+              <c:f>Hoja1!$C$12:$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -960,7 +971,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$15:$D$21</c:f>
+              <c:f>Hoja1!$D$12:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1218,9 +1229,693 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-GT">
+                <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
+              </a:rPr>
+              <a:t>Grafico</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-GT" baseline="0">
+                <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
+              </a:rPr>
+              <a:t> de Arreglos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-GT">
+              <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Showcard Gothic" panose="04020904020102020604" pitchFamily="82" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="60"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="100"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$G$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad de Arreglos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-GT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$F$12:$F$16</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Kikab</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Diego</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Alvaro</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fernando</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Emanuel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$12:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA6F-432A-83AC-655F8E31DB16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$H$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad de errores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-GT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$F$12:$F$16</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Kikab</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Diego</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Alvaro</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fernando</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Emanuel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$H$12:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA6F-432A-83AC-655F8E31DB16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:shape val="box"/>
+        <c:axId val="1769085727"/>
+        <c:axId val="1769074079"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1769085727"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769074079"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1769074079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769085727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="24">
   <a:schemeClr val="accent4"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1765,20 +2460,574 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="288">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1285874</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1803,12 +3052,48 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BCC3013-0F19-4305-9E6D-2EEB6EC627A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}" name="Tabla1" displayName="Tabla1" ref="C5:P10" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="C5:P10" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}" name="Tabla1" displayName="Tabla1" ref="C4:P9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="C4:P9" xr:uid="{89ABB43E-0AB9-4C80-9A4D-1B2B05046EF7}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{CE661E64-349B-4503-8826-B72573538F9D}" name="Equipo" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{47D53C6E-257D-4D3F-8519-A3EAC8E06F0A}" name="No. Ticket" dataDxfId="18"/>
@@ -1832,12 +3117,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}" name="Tabla2" displayName="Tabla2" ref="F14:H19" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="F14:H19" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}" name="Tabla2" displayName="Tabla2" ref="F11:H16" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="F11:H16" xr:uid="{28503D5F-B969-4E59-8D3A-1C385F58FD58}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{49D17C54-4FBB-4EEB-9308-81ECD18F5D70}" name="Developer" dataDxfId="2" dataCellStyle="20% - Énfasis4"/>
     <tableColumn id="2" xr3:uid="{BCB2DB60-3C65-4281-BC4B-E0A4D451DB4F}" name="Cantidad de Arreglos" dataDxfId="1" dataCellStyle="20% - Énfasis4"/>
-    <tableColumn id="3" xr3:uid="{85195C94-0866-4075-B0A8-863518C19B56}" name="Lineas de codigo" dataDxfId="0" dataCellStyle="20% - Énfasis4"/>
+    <tableColumn id="3" xr3:uid="{85195C94-0866-4075-B0A8-863518C19B56}" name="Cantidad de errores" dataDxfId="0" dataCellStyle="20% - Énfasis4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2140,10 +3425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8C6C0E-0565-4237-84BC-4574154DDE1B}">
-  <dimension ref="C1:R21"/>
+  <dimension ref="C1:R18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,7 +3437,7 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.42578125" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
   </cols>
@@ -2173,125 +3458,160 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+    <row r="2" spans="3:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
-    <row r="3" spans="3:18" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2">
+        <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>14</v>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
-        <v>26</v>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -2309,40 +3629,37 @@
         <v>18</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="11" t="s">
-        <v>27</v>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
+        <v>14</v>
+      </c>
+      <c r="H7" s="2">
         <v>11</v>
-      </c>
-      <c r="H7" s="2">
-        <v>7</v>
       </c>
       <c r="I7" s="2">
         <v>3</v>
       </c>
       <c r="J7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
@@ -2360,31 +3677,31 @@
         <v>18</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="11" t="s">
-        <v>22</v>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H8" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I8" s="2">
         <v>3</v>
@@ -2408,37 +3725,37 @@
         <v>18</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="11" t="s">
-        <v>28</v>
+      <c r="C9" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="2">
         <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H9" s="2">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2">
         <v>2</v>
       </c>
-      <c r="I9" s="2">
-        <v>3</v>
-      </c>
       <c r="J9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -2456,67 +3773,45 @@
         <v>18</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="2">
-        <f>SUM(Tabla1[[#This Row],[Funcionalidad ]:[Regresión ]])</f>
-        <v>14</v>
-      </c>
-      <c r="H10" s="2">
-        <v>11</v>
-      </c>
-      <c r="I10" s="2">
-        <v>2</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="10" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+    <row r="11" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2527,12 +3822,23 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="14">
+        <f>SUM(Tabla1[[Funcionalidad ]])</f>
+        <v>39</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="17">
+        <v>10</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2542,13 +3848,24 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="15">
+        <f>SUM(Tabla1[UI/UX])</f>
+        <v>13</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="18">
+        <v>11</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2558,22 +3875,23 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>35</v>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="15">
+        <f>SUM(Tabla1[Rendimiento])</f>
+        <v>2</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>38</v>
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="18">
+        <v>14</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2585,21 +3903,23 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="19">
-        <f>SUM(Tabla1[[Funcionalidad ]])</f>
-        <v>39</v>
+      <c r="D15" s="15">
+        <f>SUM(Tabla1[[Usabilidad ]])</f>
+        <v>0</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="12" t="s">
-        <v>30</v>
+      <c r="F15" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="22"/>
+        <v>4</v>
+      </c>
+      <c r="H15" s="18">
+        <v>5</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2609,22 +3929,24 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="20">
-        <f>SUM(Tabla1[UI/UX])</f>
-        <v>13</v>
+    <row r="16" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="15">
+        <f>SUM(Tabla1[DB])</f>
+        <v>0</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23"/>
+      <c r="F16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="22">
+        <v>14</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2634,139 +3956,58 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="20">
-        <f>SUM(Tabla1[Rendimiento])</f>
-        <v>2</v>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="15">
+        <f>SUM(Tabla1[Seguridad])</f>
+        <v>0</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0</v>
-      </c>
-      <c r="H17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="17" t="s">
+    <row r="18" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="20">
-        <f>SUM(Tabla1[[Usabilidad ]])</f>
+      <c r="D18" s="16">
+        <f>SUM(Tabla1[[Regresión ]])</f>
         <v>0</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0</v>
-      </c>
-      <c r="H18" s="23"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="20">
-        <f>SUM(Tabla1[DB])</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="7">
-        <v>0</v>
-      </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="20">
-        <f>SUM(Tabla1[Seguridad])</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="21">
-        <f>SUM(Tabla1[[Regresión ]])</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C2:P2"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O6" r:id="rId1" xr:uid="{5560224C-3E15-49C6-81F9-3CEE10D6C3B3}"/>
-    <hyperlink ref="P6" r:id="rId2" xr:uid="{BBEBFAB8-D149-40BE-8016-BFE5A5D9F186}"/>
-    <hyperlink ref="O7" r:id="rId3" xr:uid="{F3AF893F-D067-4B3B-BDE0-F36C80FD6E70}"/>
-    <hyperlink ref="O8" r:id="rId4" xr:uid="{50BE17E2-9FF7-4781-A7FF-EB52709B70AF}"/>
-    <hyperlink ref="O9" r:id="rId5" xr:uid="{B8BDCB57-65D4-4F7C-A9A1-39C1F27D8996}"/>
-    <hyperlink ref="O10" r:id="rId6" xr:uid="{193A4A41-A690-4106-863B-82A813D70630}"/>
-    <hyperlink ref="P7" r:id="rId7" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{5917331A-7119-4C48-A099-82561DD5A944}"/>
-    <hyperlink ref="P8" r:id="rId8" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{6A8F8094-C0E8-43F7-8AEF-9834D3AB8998}"/>
-    <hyperlink ref="P9" r:id="rId9" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{5427F53D-697E-4965-8635-AE7F542DA688}"/>
-    <hyperlink ref="P10" r:id="rId10" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{85577ADD-59C0-44E2-8D8B-1F9859167817}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{5560224C-3E15-49C6-81F9-3CEE10D6C3B3}"/>
+    <hyperlink ref="P5" r:id="rId2" xr:uid="{BBEBFAB8-D149-40BE-8016-BFE5A5D9F186}"/>
+    <hyperlink ref="O6" r:id="rId3" xr:uid="{F3AF893F-D067-4B3B-BDE0-F36C80FD6E70}"/>
+    <hyperlink ref="O7" r:id="rId4" xr:uid="{50BE17E2-9FF7-4781-A7FF-EB52709B70AF}"/>
+    <hyperlink ref="O8" r:id="rId5" xr:uid="{B8BDCB57-65D4-4F7C-A9A1-39C1F27D8996}"/>
+    <hyperlink ref="O9" r:id="rId6" xr:uid="{193A4A41-A690-4106-863B-82A813D70630}"/>
+    <hyperlink ref="P6" r:id="rId7" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{5917331A-7119-4C48-A099-82561DD5A944}"/>
+    <hyperlink ref="P7" r:id="rId8" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{6A8F8094-C0E8-43F7-8AEF-9834D3AB8998}"/>
+    <hyperlink ref="P8" r:id="rId9" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{5427F53D-697E-4965-8635-AE7F542DA688}"/>
+    <hyperlink ref="P9" r:id="rId10" display="https://boardwsactic.atlassian.net/jira/software/projects/POK/boards/2" xr:uid="{85577ADD-59C0-44E2-8D8B-1F9859167817}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>